<commit_message>
update after running test with integers set to 2 & 5
</commit_message>
<xml_diff>
--- a/CH12/Row-Inserter/insertedsplitme.xlsx
+++ b/CH12/Row-Inserter/insertedsplitme.xlsx
@@ -258,7 +258,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -355,74 +355,90 @@
       <c r="F5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Split ^^^</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Split ^^^</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>